<commit_message>
Ricompilato file report-checklist.xlsx, come da versione 4.1
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/CONCERTO/22.1.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/CONCERTO/22.1.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dedalus\GIT\it-fse-accreditamento\GATEWAY\S1#111DEDALUS0000\DEDALUS_SPA\CONCERTO\22.1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAD277E-A1D2-4996-9E90-159B95E481E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46694DC7-01CE-4261-810D-396CCD9D502D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="217" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="385">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -2680,6 +2680,21 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2701,21 +2716,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4087,10 +4087,10 @@
   <dimension ref="A1:O992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="H41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="M47" sqref="M47"/>
+      <selection pane="bottomRight" activeCell="N63" sqref="N63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -4126,14 +4126,14 @@
       <c r="O1" s="6"/>
     </row>
     <row r="2" spans="1:15" ht="18.75">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="86" t="s">
+      <c r="B2" s="90"/>
+      <c r="C2" s="91" t="s">
         <v>322</v>
       </c>
-      <c r="D2" s="85"/>
+      <c r="D2" s="90"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -4146,14 +4146,14 @@
       <c r="O2" s="6"/>
     </row>
     <row r="3" spans="1:15" ht="15.75">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="93" t="s">
+      <c r="B3" s="93"/>
+      <c r="C3" s="98" t="s">
         <v>327</v>
       </c>
-      <c r="D3" s="85"/>
+      <c r="D3" s="90"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -4166,12 +4166,12 @@
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" ht="15.75">
-      <c r="A4" s="89"/>
-      <c r="B4" s="90"/>
-      <c r="C4" s="93" t="s">
+      <c r="A4" s="94"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="98" t="s">
         <v>323</v>
       </c>
-      <c r="D4" s="85"/>
+      <c r="D4" s="90"/>
       <c r="E4" s="2"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -4185,12 +4185,12 @@
       <c r="O4" s="6"/>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="91"/>
-      <c r="B5" s="92"/>
-      <c r="C5" s="93" t="s">
+      <c r="A5" s="96"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="98" t="s">
         <v>328</v>
       </c>
-      <c r="D5" s="85"/>
+      <c r="D5" s="90"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -4203,8 +4203,8 @@
       <c r="O5" s="6"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="82"/>
-      <c r="B6" s="83"/>
+      <c r="A6" s="87"/>
+      <c r="B6" s="88"/>
       <c r="C6" s="10"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -4284,7 +4284,7 @@
       <c r="M9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="94" t="s">
+      <c r="N9" s="82" t="s">
         <v>23</v>
       </c>
       <c r="O9" s="12" t="s">
@@ -4327,7 +4327,7 @@
         <v>319</v>
       </c>
       <c r="M10" s="45"/>
-      <c r="N10" s="95"/>
+      <c r="N10" s="83"/>
       <c r="O10" s="73"/>
     </row>
     <row r="11" spans="1:15" s="47" customFormat="1" ht="241.9" customHeight="1" thickBot="1">
@@ -4366,7 +4366,7 @@
         <v>319</v>
       </c>
       <c r="M11" s="45"/>
-      <c r="N11" s="95"/>
+      <c r="N11" s="83"/>
       <c r="O11" s="49"/>
     </row>
     <row r="12" spans="1:15" s="47" customFormat="1" ht="241.9" customHeight="1" thickBot="1">
@@ -4405,7 +4405,7 @@
         <v>319</v>
       </c>
       <c r="M12" s="45"/>
-      <c r="N12" s="95"/>
+      <c r="N12" s="83"/>
       <c r="O12" s="49"/>
     </row>
     <row r="13" spans="1:15" s="47" customFormat="1" ht="241.9" customHeight="1" thickBot="1">
@@ -4444,7 +4444,7 @@
         <v>319</v>
       </c>
       <c r="M13" s="45"/>
-      <c r="N13" s="95"/>
+      <c r="N13" s="83"/>
       <c r="O13" s="70"/>
     </row>
     <row r="14" spans="1:15" s="47" customFormat="1" ht="241.9" customHeight="1" thickBot="1">
@@ -4483,7 +4483,7 @@
         <v>319</v>
       </c>
       <c r="M14" s="45"/>
-      <c r="N14" s="95"/>
+      <c r="N14" s="83"/>
       <c r="O14" s="72"/>
     </row>
     <row r="15" spans="1:15" ht="409.6" hidden="1" thickBot="1">
@@ -5064,7 +5064,9 @@
         <v>319</v>
       </c>
       <c r="M35" s="45"/>
-      <c r="N35" s="95"/>
+      <c r="N35" s="83" t="s">
+        <v>84</v>
+      </c>
       <c r="O35" s="46" t="s">
         <v>345</v>
       </c>
@@ -5252,7 +5254,9 @@
         <v>319</v>
       </c>
       <c r="M41" s="45"/>
-      <c r="N41" s="95"/>
+      <c r="N41" s="83" t="s">
+        <v>84</v>
+      </c>
       <c r="O41" s="46" t="s">
         <v>349</v>
       </c>
@@ -5432,7 +5436,7 @@
       </c>
       <c r="L47" s="45"/>
       <c r="M47" s="45"/>
-      <c r="N47" s="95" t="s">
+      <c r="N47" s="83" t="s">
         <v>84</v>
       </c>
       <c r="O47" s="49"/>
@@ -5620,7 +5624,9 @@
         <v>319</v>
       </c>
       <c r="M53" s="57"/>
-      <c r="N53" s="96"/>
+      <c r="N53" s="84" t="s">
+        <v>84</v>
+      </c>
       <c r="O53" s="81" t="s">
         <v>377</v>
       </c>
@@ -5663,7 +5669,9 @@
         <v>319</v>
       </c>
       <c r="M54" s="65"/>
-      <c r="N54" s="97"/>
+      <c r="N54" s="85" t="s">
+        <v>84</v>
+      </c>
       <c r="O54" s="74" t="s">
         <v>356</v>
       </c>
@@ -5706,7 +5714,9 @@
         <v>319</v>
       </c>
       <c r="M55" s="18"/>
-      <c r="N55" s="19"/>
+      <c r="N55" s="19" t="s">
+        <v>84</v>
+      </c>
       <c r="O55" s="80" t="s">
         <v>360</v>
       </c>
@@ -5749,7 +5759,9 @@
         <v>319</v>
       </c>
       <c r="M56" s="18"/>
-      <c r="N56" s="19"/>
+      <c r="N56" s="19" t="s">
+        <v>84</v>
+      </c>
       <c r="O56" s="80" t="s">
         <v>364</v>
       </c>
@@ -5784,7 +5796,9 @@
       <c r="M57" s="56" t="s">
         <v>325</v>
       </c>
-      <c r="N57" s="98"/>
+      <c r="N57" s="86" t="s">
+        <v>84</v>
+      </c>
       <c r="O57" s="58"/>
     </row>
     <row r="58" spans="1:15" ht="241.9" customHeight="1" thickBot="1">
@@ -5825,7 +5839,9 @@
         <v>319</v>
       </c>
       <c r="M58" s="18"/>
-      <c r="N58" s="19"/>
+      <c r="N58" s="19" t="s">
+        <v>84</v>
+      </c>
       <c r="O58" s="80" t="s">
         <v>368</v>
       </c>
@@ -5868,7 +5884,9 @@
         <v>319</v>
       </c>
       <c r="M59" s="18"/>
-      <c r="N59" s="19"/>
+      <c r="N59" s="19" t="s">
+        <v>84</v>
+      </c>
       <c r="O59" s="80" t="s">
         <v>372</v>
       </c>
@@ -5903,7 +5921,9 @@
       <c r="M60" s="56" t="s">
         <v>324</v>
       </c>
-      <c r="N60" s="98"/>
+      <c r="N60" s="86" t="s">
+        <v>84</v>
+      </c>
       <c r="O60" s="58"/>
     </row>
     <row r="61" spans="1:15" ht="241.9" customHeight="1" thickBot="1">
@@ -5944,7 +5964,9 @@
         <v>319</v>
       </c>
       <c r="M61" s="18"/>
-      <c r="N61" s="19"/>
+      <c r="N61" s="19" t="s">
+        <v>84</v>
+      </c>
       <c r="O61" s="80" t="s">
         <v>376</v>
       </c>
@@ -5985,7 +6007,9 @@
         <v>319</v>
       </c>
       <c r="M62" s="18"/>
-      <c r="N62" s="19"/>
+      <c r="N62" s="19" t="s">
+        <v>84</v>
+      </c>
       <c r="O62" s="20" t="s">
         <v>384</v>
       </c>
@@ -6020,7 +6044,9 @@
       <c r="M63" s="56" t="s">
         <v>326</v>
       </c>
-      <c r="N63" s="98"/>
+      <c r="N63" s="86" t="s">
+        <v>84</v>
+      </c>
       <c r="O63" s="58"/>
     </row>
     <row r="64" spans="1:15" ht="345" hidden="1">

</xml_diff>

<commit_message>
Caso 56: Eliminata colonna F perchè non applicabile Caso 59: Eliminata colonna F perchè non applicabile Caso 62: Eliminata colonna F perchè non applicabile Caso 61: Popolata colonna J con la gestione errore
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/CONCERTO/22.1.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/CONCERTO/22.1.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dedalus\GIT\it-fse-accreditamento\GATEWAY\S1#111DEDALUS0000\DEDALUS_SPA\CONCERTO\22.1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46694DC7-01CE-4261-810D-396CCD9D502D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E736B18-2C7E-4A97-BEEF-3CF0D27903E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="217" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="386">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -1974,6 +1974,11 @@
   </si>
   <si>
     <t xml:space="preserve">Lo specimenPlayingEntity contiene solo l'elemento id e non l'elemento code,ma non otteniamo errore: Il pdf viene accettato senza errori.  Nel CDA di Concerto ci sarà sempre l'elemento specimen/specimenRole/id. Quello sottomesso è l'unico caso gestibile. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In caso venga restituito un errore:
+- il programma di firma digitale presidiata mostra un messaggio a video con l'errore che proviene dal servizio di validazione. Il messaggio è memorizzato per analisi successiva in backoffice. 
+- il programma di firma digitale non presidiata memorizza il messaggio di errore che proviene dal servizio di validazione per analisi successiva in backoffice. </t>
   </si>
 </sst>
 </file>
@@ -4087,10 +4092,10 @@
   <dimension ref="A1:O992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="N63" sqref="N63"/>
+      <selection pane="bottomRight" activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -5782,9 +5787,7 @@
       <c r="E57" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="F57" s="40">
-        <v>44980</v>
-      </c>
+      <c r="F57" s="40"/>
       <c r="G57" s="53"/>
       <c r="H57" s="53"/>
       <c r="I57" s="55"/>
@@ -5907,9 +5910,7 @@
       <c r="E60" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="F60" s="40">
-        <v>44980</v>
-      </c>
+      <c r="F60" s="40"/>
       <c r="G60" s="53"/>
       <c r="H60" s="53"/>
       <c r="I60" s="55"/>
@@ -5999,7 +6000,9 @@
       <c r="I62" s="37" t="s">
         <v>383</v>
       </c>
-      <c r="J62" s="44"/>
+      <c r="J62" s="44" t="s">
+        <v>385</v>
+      </c>
       <c r="K62" s="18" t="s">
         <v>84</v>
       </c>
@@ -6030,9 +6033,7 @@
       <c r="E63" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="F63" s="40">
-        <v>44980</v>
-      </c>
+      <c r="F63" s="40"/>
       <c r="G63" s="53"/>
       <c r="H63" s="53"/>
       <c r="I63" s="55"/>

</xml_diff>

<commit_message>
Eseguite modifiche segnalate : Modificato data.json riportando i file corretti; Aggiornato file CASO_4_OK.pdf e rieseguito Upload per aggiunta methodCode: riaggiornato data.json e report-checklist.xlsx per il test rieseguito
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/CONCERTO/22.1.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/CONCERTO/22.1.0/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dedalus\GIT\it-fse-accreditamento\GATEWAY\S1#111DEDALUS0000\DEDALUS_SPA\CONCERTO\22.1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E736B18-2C7E-4A97-BEEF-3CF0D27903E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035B8827-08AC-478B-BE89-62F1AC827630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="217" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="387">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -1958,9 +1958,6 @@
     <t>2023-02-23T17:00:29Z</t>
   </si>
   <si>
-    <t>2ac15f899768c0cd</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.50912.4.4.1.6fcfadf5232d0c1c1e5316eaa3c5f1c5c03d08d2b480f0e6559ec58328f62594.6a1e197e3b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
@@ -1979,6 +1976,12 @@
     <t xml:space="preserve">In caso venga restituito un errore:
 - il programma di firma digitale presidiata mostra un messaggio a video con l'errore che proviene dal servizio di validazione. Il messaggio è memorizzato per analisi successiva in backoffice. 
 - il programma di firma digitale non presidiata memorizza il messaggio di errore che proviene dal servizio di validazione per analisi successiva in backoffice. </t>
+  </si>
+  <si>
+    <t>1664091f8f0caf58</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50912.4.4.1.78e8e13ebc6af0ade63564b47c10352491fb2eeae641311148582846cfcac518.3e0e498c71^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4092,10 +4095,10 @@
   <dimension ref="A1:O992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J62" sqref="J62"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -4430,16 +4433,16 @@
         <v>34</v>
       </c>
       <c r="F13" s="40">
-        <v>44980</v>
+        <v>45014</v>
       </c>
       <c r="G13" s="42" t="s">
         <v>378</v>
       </c>
       <c r="H13" s="42" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="I13" s="43" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="J13" s="45"/>
       <c r="K13" s="45" t="s">
@@ -5992,16 +5995,16 @@
         <v>44980</v>
       </c>
       <c r="G62" s="17" t="s">
+        <v>380</v>
+      </c>
+      <c r="H62" s="17" t="s">
         <v>381</v>
       </c>
-      <c r="H62" s="17" t="s">
+      <c r="I62" s="37" t="s">
         <v>382</v>
       </c>
-      <c r="I62" s="37" t="s">
-        <v>383</v>
-      </c>
       <c r="J62" s="44" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K62" s="18" t="s">
         <v>84</v>
@@ -6014,7 +6017,7 @@
         <v>84</v>
       </c>
       <c r="O62" s="20" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="63" spans="1:15" s="59" customFormat="1" ht="241.9" customHeight="1">

</xml_diff>